<commit_message>
Created: updated FSEOF for GSM
</commit_message>
<xml_diff>
--- a/ecYaliGEM/output/enzymeUsage vs FSEOF.xlsx
+++ b/ecYaliGEM/output/enzymeUsage vs FSEOF.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ECDCB8-94DF-42F6-BEBE-18F192312CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F8DD06-9CEB-4059-8E40-0F294F8ECF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2400" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ecYali" sheetId="1" r:id="rId1"/>
     <sheet name="ecYali_Nlim" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
-    <sheet name="iYali" sheetId="5" r:id="rId4"/>
-    <sheet name="NGAM plot" sheetId="2" r:id="rId5"/>
-    <sheet name="prot_pool plot" sheetId="4" r:id="rId6"/>
+    <sheet name="iYali" sheetId="5" r:id="rId3"/>
+    <sheet name="NGAM plot" sheetId="2" r:id="rId4"/>
+    <sheet name="prot_pool plot" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="877">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="880">
   <si>
     <t>'y000027'</t>
   </si>
@@ -2672,16 +2671,26 @@
   </si>
   <si>
     <t>y000907_EXP_1'</t>
+  </si>
+  <si>
+    <t>Q6C3Z9'</t>
+  </si>
+  <si>
+    <t>y000111'</t>
+  </si>
+  <si>
+    <t>Q6C1X5'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="170" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -2771,7 +2780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2804,6 +2813,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2846,7 +2856,12 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -2855,12 +2870,7 @@
       <numFmt numFmtId="165" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -5206,6 +5216,539 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ecYali (generic) simulations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'prot_pool plot'!$D$18:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.23150023150023127</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25565430762641872</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.27980838375260614</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30396245987879356</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32811653600498097</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35227061213116845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.37642468825735587</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.40057876438354328</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.42473284050972959</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.44888691663591701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.47304099276210443</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.49719506888829185</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.52134914501447926</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.54550322114066674</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5696572972668541</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.59381137339304157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'prot_pool plot'!$E$18:$E$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.0E+00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2.3457164409083401E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4988631091477602E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.65864406400896E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.81788879572254E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9811512714768301E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1413243694823899E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.30461132894369E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4714801734404003E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.6377296230064601E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.8039790725525702E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9737671375053102E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1412025412970298E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.3086379450940198E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.4730108493346802E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9418278341635699E-4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.5692457080299298E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3B24-4F89-B71D-2317B6126669}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="47624192"/>
+        <c:axId val="1730146080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="47624192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.60000000000000009"/>
+          <c:min val="0.2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Ysx</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1730146080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1730146080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Specific</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> lipid production (mmol/g</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="-25000"/>
+                  <a:t>DCW</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t>.h)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="47624192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5247,6 +5790,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6318,6 +6901,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6399,6 +7498,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{071AC44C-ACE9-94CB-F835-5F2BA9D6F8F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6444,13 +7579,7 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C6AE83F6-0BCA-4846-8A86-50B0E87B7071}" name="Tabela4" displayName="Tabela4" ref="A2:H29" totalsRowShown="0">
-  <autoFilter ref="A2:H29" xr:uid="{C6AE83F6-0BCA-4846-8A86-50B0E87B7071}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="0"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:H29" xr:uid="{C6AE83F6-0BCA-4846-8A86-50B0E87B7071}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H29">
     <sortCondition ref="C2:C29"/>
   </sortState>
@@ -6523,14 +7652,14 @@
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{4905A0A7-9CA0-4B61-A17A-A60AA93CFAF9}" name="protID"/>
     <tableColumn id="2" xr3:uid="{07CE7141-993F-4265-ADA2-1D7AE02E2331}" name="geneID"/>
-    <tableColumn id="3" xr3:uid="{DD485713-254D-456F-A6A4-FF80A9F2504A}" name="absUsage" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{6ED1EEFA-F296-4FEE-8090-465370BDD4EB}" name="percUsage" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{8EF813D8-C987-4BEE-BB29-271B2A5ADA14}" name="kcat" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{DD485713-254D-456F-A6A4-FF80A9F2504A}" name="absUsage" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{6ED1EEFA-F296-4FEE-8090-465370BDD4EB}" name="percUsage" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{8EF813D8-C987-4BEE-BB29-271B2A5ADA14}" name="kcat" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{E9482A6E-4578-462E-B118-408E2D0DD4F9}" name="sorce"/>
     <tableColumn id="7" xr3:uid="{3318B392-664A-4D18-A77D-DFA08B424AEA}" name="rxnID"/>
     <tableColumn id="8" xr3:uid="{54DDE929-E8C8-4736-9AD2-5FD58FCAE634}" name="rxnNames"/>
     <tableColumn id="9" xr3:uid="{44B3321F-81D2-4832-A9C4-ED4925AE4EEB}" name="grRules"/>
-    <tableColumn id="10" xr3:uid="{0A4F1D80-C65F-4E35-8820-A1CCE3DCC85B}" name="FSEOF?" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{0A4F1D80-C65F-4E35-8820-A1CCE3DCC85B}" name="FSEOF?" dataDxfId="6">
       <calculatedColumnFormula>COUNTIF(Tabela5[rxnID],G83)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{84091260-CE60-469A-9EF2-267494370C4C}" name="Full capacity?">
@@ -6832,7 +7961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA156"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -13591,8 +14720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD147150-DDDE-4176-9567-786D2C29D3F7}">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67"/>
+    <sheetView topLeftCell="H16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13666,8 +14795,8 @@
       <c r="B3" t="s">
         <v>85</v>
       </c>
-      <c r="C3" t="s">
-        <v>86</v>
+      <c r="C3" s="3" t="s">
+        <v>875</v>
       </c>
       <c r="D3" t="s">
         <v>87</v>
@@ -13714,8 +14843,8 @@
       <c r="B4" t="s">
         <v>89</v>
       </c>
-      <c r="C4" t="s">
-        <v>86</v>
+      <c r="C4" s="3" t="s">
+        <v>875</v>
       </c>
       <c r="D4" t="s">
         <v>87</v>
@@ -14047,15 +15176,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" t="s">
-        <v>12</v>
+      <c r="C15" s="3" t="s">
+        <v>879</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -14071,10 +15200,10 @@
       </c>
       <c r="H15">
         <f>COUNTIF($K$4:$K$5,Tabela4[[#This Row],[protID]])</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" hidden="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -14101,7 +15230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -14128,7 +15257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>207</v>
       </c>
@@ -14155,7 +15284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>209</v>
       </c>
@@ -14183,14 +15312,14 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" t="s">
-        <v>24</v>
+      <c r="A20" s="3" t="s">
+        <v>878</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="C20" t="s">
-        <v>26</v>
+      <c r="C20" s="3" t="s">
+        <v>877</v>
       </c>
       <c r="D20" t="s">
         <v>27</v>
@@ -16385,163 +17514,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84BD11D-D0CD-411C-ADEC-58DC597399F3}">
-  <dimension ref="A1:L19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="B4">
-        <v>4.7417790265767701E-3</v>
-      </c>
-      <c r="C4" s="6">
-        <v>3.09500869934083E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="B5">
-        <v>5.6901348318921302E-3</v>
-      </c>
-      <c r="C5" s="6">
-        <v>3.71435635208402E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="B6">
-        <v>6.6384906372074799E-3</v>
-      </c>
-      <c r="C6" s="6">
-        <v>4.3337040048175302E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="B7">
-        <v>7.5868464425228399E-3</v>
-      </c>
-      <c r="C7" s="6">
-        <v>4.9530516575521401E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="B8">
-        <v>8.5352022478381896E-3</v>
-      </c>
-      <c r="C8" s="6">
-        <v>5.5723993102942799E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="B9">
-        <v>9.4835580531535402E-3</v>
-      </c>
-      <c r="C9" s="6">
-        <v>6.1919656017536695E-5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="B10">
-        <v>1.0431913858468899E-2</v>
-      </c>
-      <c r="C10" s="6">
-        <v>6.8123626098722195E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="B11">
-        <v>1.13802696637843E-2</v>
-      </c>
-      <c r="C11" s="6">
-        <v>7.4248103026877595E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="B12">
-        <v>1.23286254690996E-2</v>
-      </c>
-      <c r="C12" s="6">
-        <v>7.8936558082373206E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="B13">
-        <v>1.3276981274415E-2</v>
-      </c>
-      <c r="C13" s="6">
-        <v>8.4452725478798994E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="B14">
-        <v>1.42253370797303E-2</v>
-      </c>
-      <c r="C14" s="6">
-        <v>9.0552198703544405E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="B15">
-        <v>1.5173692885045701E-2</v>
-      </c>
-      <c r="C15" s="6">
-        <v>9.6651790669485701E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="B16">
-        <v>1.6122048690361001E-2</v>
-      </c>
-      <c r="C16">
-        <v>1.02751382635302E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17">
-        <v>1.70704044956764E-2</v>
-      </c>
-      <c r="C17">
-        <v>1.08853621455825E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18">
-        <v>1.8018760300991699E-2</v>
-      </c>
-      <c r="C18">
-        <v>1.14956658016229E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19">
-        <v>1.8967116106307101E-2</v>
-      </c>
-      <c r="C19">
-        <v>1.21059694576273E-4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643171A4-4CC4-44B6-8A09-51199A818DEA}">
   <dimension ref="A1:J62"/>
   <sheetViews>
@@ -17938,7 +18910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D90E3B-8D28-4790-BCAD-AF23A4BA39F8}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -18299,12 +19271,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712D4235-63CA-46AD-95AB-3CF58DD6FAD4}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18812,6 +19784,134 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="4:5">
+      <c r="D18">
+        <v>0.23150023150023127</v>
+      </c>
+      <c r="E18" s="24">
+        <v>2.3457164409083401E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5">
+      <c r="D19">
+        <v>0.25565430762641872</v>
+      </c>
+      <c r="E19" s="24">
+        <v>2.4988631091477602E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="D20">
+        <v>0.27980838375260614</v>
+      </c>
+      <c r="E20" s="24">
+        <v>2.65864406400896E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5">
+      <c r="D21">
+        <v>0.30396245987879356</v>
+      </c>
+      <c r="E21" s="24">
+        <v>2.81788879572254E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5">
+      <c r="D22">
+        <v>0.32811653600498097</v>
+      </c>
+      <c r="E22" s="24">
+        <v>2.9811512714768301E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5">
+      <c r="D23">
+        <v>0.35227061213116845</v>
+      </c>
+      <c r="E23" s="24">
+        <v>3.1413243694823899E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5">
+      <c r="D24">
+        <v>0.37642468825735587</v>
+      </c>
+      <c r="E24" s="24">
+        <v>3.30461132894369E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5">
+      <c r="D25">
+        <v>0.40057876438354328</v>
+      </c>
+      <c r="E25" s="24">
+        <v>3.4714801734404003E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5">
+      <c r="D26">
+        <v>0.42473284050972959</v>
+      </c>
+      <c r="E26" s="24">
+        <v>3.6377296230064601E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5">
+      <c r="D27">
+        <v>0.44888691663591701</v>
+      </c>
+      <c r="E27" s="24">
+        <v>3.8039790725525702E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5">
+      <c r="D28">
+        <v>0.47304099276210443</v>
+      </c>
+      <c r="E28" s="24">
+        <v>3.9737671375053102E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5">
+      <c r="D29">
+        <v>0.49719506888829185</v>
+      </c>
+      <c r="E29" s="24">
+        <v>4.1412025412970298E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5">
+      <c r="D30">
+        <v>0.52134914501447926</v>
+      </c>
+      <c r="E30" s="24">
+        <v>4.3086379450940198E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5">
+      <c r="D31">
+        <v>0.54550322114066674</v>
+      </c>
+      <c r="E31" s="24">
+        <v>4.4730108493346802E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5">
+      <c r="D32">
+        <v>0.5696572972668541</v>
+      </c>
+      <c r="E32" s="24">
+        <v>3.9418278341635699E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5">
+      <c r="D33">
+        <v>0.59381137339304157</v>
+      </c>
+      <c r="E33" s="24">
+        <v>3.5692457080299298E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Edit: FCC script - fine tuned parameters
</commit_message>
<xml_diff>
--- a/ecYaliGEM/output/enzymeUsage vs FSEOF.xlsx
+++ b/ecYaliGEM/output/enzymeUsage vs FSEOF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jujum\OneDrive\Documentos\GitHub\GECKO\ecYaliGEM\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100F1843-FDCE-44B1-AE7D-C9ED553EC8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4000D30-67C9-40C2-8FE3-5B9B58A7EACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3650" yWindow="14290" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ecYali" sheetId="1" r:id="rId1"/>
@@ -5638,6 +5638,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5649,16 +5659,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5806,7 +5806,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6892,7 +6892,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -8068,7 +8068,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10863,37 +10863,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>642</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="K1" s="23" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="K1" s="27" t="s">
         <v>643</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="U1" s="24" t="s">
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="U1" s="28" t="s">
         <v>847</v>
       </c>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -16485,14 +16485,14 @@
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A105" s="21" t="s">
+      <c r="A105" s="25" t="s">
         <v>732</v>
       </c>
-      <c r="B105" s="21"/>
-      <c r="C105" s="21"/>
-      <c r="D105" s="21"/>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
+      <c r="B105" s="25"/>
+      <c r="C105" s="25"/>
+      <c r="D105" s="25"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="25"/>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
@@ -17625,16 +17625,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>642</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -17661,15 +17661,15 @@
       <c r="H2" t="s">
         <v>423</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="28" t="s">
         <v>873</v>
       </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -18466,15 +18466,15 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="25" t="s">
         <v>732</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -19469,19 +19469,19 @@
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="23" t="s">
+      <c r="A81" s="27" t="s">
         <v>802</v>
       </c>
-      <c r="B81" s="23"/>
-      <c r="C81" s="23"/>
-      <c r="D81" s="23"/>
-      <c r="E81" s="23"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="23"/>
-      <c r="H81" s="23"/>
-      <c r="I81" s="23"/>
-      <c r="J81" s="23"/>
-      <c r="K81" s="23"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="27"/>
+      <c r="I81" s="27"/>
+      <c r="J81" s="27"/>
+      <c r="K81" s="27"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
@@ -20400,7 +20400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643171A4-4CC4-44B6-8A09-51199A818DEA}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -20417,16 +20417,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>637</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -22158,8 +22158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712D4235-63CA-46AD-95AB-3CF58DD6FAD4}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F17" sqref="C17:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27822,10 +27822,10 @@
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A280" s="25" t="s">
+      <c r="A280" s="21" t="s">
         <v>1506</v>
       </c>
-      <c r="B280" s="25" t="s">
+      <c r="B280" s="21" t="s">
         <v>1574</v>
       </c>
       <c r="C280" t="s">
@@ -27839,7 +27839,7 @@
       <c r="B281" t="s">
         <v>451</v>
       </c>
-      <c r="C281" s="26">
+      <c r="C281" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27850,7 +27850,7 @@
       <c r="B282" t="s">
         <v>890</v>
       </c>
-      <c r="C282" s="26">
+      <c r="C282" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27861,7 +27861,7 @@
       <c r="B283" t="s">
         <v>887</v>
       </c>
-      <c r="C283" s="26">
+      <c r="C283" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27872,7 +27872,7 @@
       <c r="B284" t="s">
         <v>793</v>
       </c>
-      <c r="C284" s="26">
+      <c r="C284" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27883,7 +27883,7 @@
       <c r="B285" t="s">
         <v>47</v>
       </c>
-      <c r="C285" s="26">
+      <c r="C285" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27894,7 +27894,7 @@
       <c r="B286" t="s">
         <v>320</v>
       </c>
-      <c r="C286" s="26">
+      <c r="C286" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27905,7 +27905,7 @@
       <c r="B287" t="s">
         <v>373</v>
       </c>
-      <c r="C287" s="26">
+      <c r="C287" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27916,7 +27916,7 @@
       <c r="B288" t="s">
         <v>373</v>
       </c>
-      <c r="C288" s="26">
+      <c r="C288" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27927,7 +27927,7 @@
       <c r="B289" t="s">
         <v>47</v>
       </c>
-      <c r="C289" s="26">
+      <c r="C289" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27938,7 +27938,7 @@
       <c r="B290" t="s">
         <v>320</v>
       </c>
-      <c r="C290" s="26">
+      <c r="C290" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27949,7 +27949,7 @@
       <c r="B291" t="s">
         <v>218</v>
       </c>
-      <c r="C291" s="26">
+      <c r="C291" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27960,7 +27960,7 @@
       <c r="B292" t="s">
         <v>218</v>
       </c>
-      <c r="C292" s="26">
+      <c r="C292" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27971,7 +27971,7 @@
       <c r="B293" t="s">
         <v>47</v>
       </c>
-      <c r="C293" s="26">
+      <c r="C293" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27982,7 +27982,7 @@
       <c r="B294" t="s">
         <v>218</v>
       </c>
-      <c r="C294" s="26">
+      <c r="C294" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -27993,7 +27993,7 @@
       <c r="B295" t="s">
         <v>218</v>
       </c>
-      <c r="C295" s="26">
+      <c r="C295" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -28004,7 +28004,7 @@
       <c r="B296" t="s">
         <v>47</v>
       </c>
-      <c r="C296" s="26">
+      <c r="C296" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -28015,7 +28015,7 @@
       <c r="B297" t="s">
         <v>218</v>
       </c>
-      <c r="C297" s="26">
+      <c r="C297" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -28026,7 +28026,7 @@
       <c r="B298" t="s">
         <v>218</v>
       </c>
-      <c r="C298" s="26">
+      <c r="C298" s="22">
         <v>1000</v>
       </c>
     </row>
@@ -28037,7 +28037,7 @@
       <c r="B299" t="s">
         <v>915</v>
       </c>
-      <c r="C299" s="27">
+      <c r="C299" s="23">
         <v>37.259538391246998</v>
       </c>
     </row>
@@ -28048,7 +28048,7 @@
       <c r="B300" t="s">
         <v>921</v>
       </c>
-      <c r="C300" s="27">
+      <c r="C300" s="23">
         <v>23.570006411903901</v>
       </c>
     </row>
@@ -28059,7 +28059,7 @@
       <c r="B301" s="10" t="s">
         <v>918</v>
       </c>
-      <c r="C301" s="28">
+      <c r="C301" s="24">
         <v>23.570006411903901</v>
       </c>
     </row>
@@ -28070,7 +28070,7 @@
       <c r="B302" t="s">
         <v>934</v>
       </c>
-      <c r="C302" s="27">
+      <c r="C302" s="23">
         <v>8.3361576667160104</v>
       </c>
     </row>
@@ -28081,7 +28081,7 @@
       <c r="B303" t="s">
         <v>928</v>
       </c>
-      <c r="C303" s="27">
+      <c r="C303" s="23">
         <v>8.3361576667160104</v>
       </c>
     </row>
@@ -28092,7 +28092,7 @@
       <c r="B304" t="s">
         <v>931</v>
       </c>
-      <c r="C304" s="27">
+      <c r="C304" s="23">
         <v>8.3361576667160104</v>
       </c>
     </row>
@@ -28103,7 +28103,7 @@
       <c r="B305" t="s">
         <v>705</v>
       </c>
-      <c r="C305" s="27">
+      <c r="C305" s="23">
         <v>8.3361576667160104</v>
       </c>
     </row>
@@ -28114,7 +28114,7 @@
       <c r="B306" t="s">
         <v>705</v>
       </c>
-      <c r="C306" s="27">
+      <c r="C306" s="23">
         <v>8.3361576667160104</v>
       </c>
     </row>
@@ -28125,7 +28125,7 @@
       <c r="B307" t="s">
         <v>705</v>
       </c>
-      <c r="C307" s="27">
+      <c r="C307" s="23">
         <v>8.3361576667160104</v>
       </c>
     </row>
@@ -28136,7 +28136,7 @@
       <c r="B308" t="s">
         <v>941</v>
       </c>
-      <c r="C308" s="27">
+      <c r="C308" s="23">
         <v>8.3361576667160104</v>
       </c>
     </row>
@@ -28147,7 +28147,7 @@
       <c r="B309" t="s">
         <v>959</v>
       </c>
-      <c r="C309" s="27">
+      <c r="C309" s="23">
         <v>8.3361576667159802</v>
       </c>
     </row>
@@ -28158,7 +28158,7 @@
       <c r="B310" t="s">
         <v>963</v>
       </c>
-      <c r="C310" s="27">
+      <c r="C310" s="23">
         <v>8.3361576667159802</v>
       </c>
     </row>
@@ -28169,7 +28169,7 @@
       <c r="B311" t="s">
         <v>971</v>
       </c>
-      <c r="C311" s="27">
+      <c r="C311" s="23">
         <v>8.3078045578858593</v>
       </c>
     </row>
@@ -28180,7 +28180,7 @@
       <c r="B312" t="s">
         <v>971</v>
       </c>
-      <c r="C312" s="27">
+      <c r="C312" s="23">
         <v>8.3078045578858593</v>
       </c>
     </row>
@@ -28191,7 +28191,7 @@
       <c r="B313" t="s">
         <v>968</v>
       </c>
-      <c r="C313" s="27">
+      <c r="C313" s="23">
         <v>8.3055026910018093</v>
       </c>
     </row>
@@ -28202,7 +28202,7 @@
       <c r="B314" t="s">
         <v>968</v>
       </c>
-      <c r="C314" s="27">
+      <c r="C314" s="23">
         <v>8.3055026910018093</v>
       </c>
     </row>
@@ -28213,7 +28213,7 @@
       <c r="B315" t="s">
         <v>743</v>
       </c>
-      <c r="C315" s="27">
+      <c r="C315" s="23">
         <v>6.5895141029773301</v>
       </c>
     </row>
@@ -28224,7 +28224,7 @@
       <c r="B316" t="s">
         <v>977</v>
       </c>
-      <c r="C316" s="27">
+      <c r="C316" s="23">
         <v>6.5895141029773301</v>
       </c>
     </row>
@@ -28235,7 +28235,7 @@
       <c r="B317" t="s">
         <v>977</v>
       </c>
-      <c r="C317" s="27">
+      <c r="C317" s="23">
         <v>6.5895141029773301</v>
       </c>
     </row>
@@ -28246,7 +28246,7 @@
       <c r="B318" t="s">
         <v>313</v>
       </c>
-      <c r="C318" s="27">
+      <c r="C318" s="23">
         <v>6.3879103274026097</v>
       </c>
     </row>
@@ -28257,7 +28257,7 @@
       <c r="B319" t="s">
         <v>313</v>
       </c>
-      <c r="C319" s="27">
+      <c r="C319" s="23">
         <v>6.3879103274026097</v>
       </c>
     </row>
@@ -28268,7 +28268,7 @@
       <c r="B320" t="s">
         <v>313</v>
       </c>
-      <c r="C320" s="27">
+      <c r="C320" s="23">
         <v>6.3879103274026097</v>
       </c>
     </row>
@@ -28279,7 +28279,7 @@
       <c r="B321" t="s">
         <v>313</v>
       </c>
-      <c r="C321" s="27">
+      <c r="C321" s="23">
         <v>6.3879103274026097</v>
       </c>
     </row>
@@ -28290,7 +28290,7 @@
       <c r="B322" t="s">
         <v>348</v>
       </c>
-      <c r="C322" s="27">
+      <c r="C322" s="23">
         <v>4.1610705012346099</v>
       </c>
     </row>
@@ -28301,7 +28301,7 @@
       <c r="B323" t="s">
         <v>125</v>
       </c>
-      <c r="C323" s="27">
+      <c r="C323" s="23">
         <v>2.8663957832289002</v>
       </c>
     </row>
@@ -28312,7 +28312,7 @@
       <c r="B324" t="s">
         <v>125</v>
       </c>
-      <c r="C324" s="27">
+      <c r="C324" s="23">
         <v>2.8663957832289002</v>
       </c>
     </row>
@@ -28323,7 +28323,7 @@
       <c r="B325" t="s">
         <v>324</v>
       </c>
-      <c r="C325" s="27">
+      <c r="C325" s="23">
         <v>2.69563499860869</v>
       </c>
     </row>
@@ -28334,7 +28334,7 @@
       <c r="B326" t="s">
         <v>293</v>
       </c>
-      <c r="C326" s="27">
+      <c r="C326" s="23">
         <v>1.5200771413065499</v>
       </c>
     </row>
@@ -28345,7 +28345,7 @@
       <c r="B327" t="s">
         <v>277</v>
       </c>
-      <c r="C327" s="27">
+      <c r="C327" s="23">
         <v>1.43120263014339</v>
       </c>
     </row>
@@ -28356,7 +28356,7 @@
       <c r="B328" t="s">
         <v>273</v>
       </c>
-      <c r="C328" s="27">
+      <c r="C328" s="23">
         <v>1.43120263014339</v>
       </c>
     </row>
@@ -28367,7 +28367,7 @@
       <c r="B329" t="s">
         <v>301</v>
       </c>
-      <c r="C329" s="27">
+      <c r="C329" s="23">
         <v>1.1105322590645801</v>
       </c>
     </row>
@@ -28378,7 +28378,7 @@
       <c r="B330" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="C330" s="28">
+      <c r="C330" s="24">
         <v>1.1105322590645801</v>
       </c>
     </row>
@@ -28389,7 +28389,7 @@
       <c r="B331" t="s">
         <v>443</v>
       </c>
-      <c r="C331" s="27">
+      <c r="C331" s="23">
         <v>1.10642064740061</v>
       </c>
     </row>
@@ -28400,7 +28400,7 @@
       <c r="B332" t="s">
         <v>447</v>
       </c>
-      <c r="C332" s="27">
+      <c r="C332" s="23">
         <v>1.10642064740061</v>
       </c>
     </row>
@@ -28411,7 +28411,7 @@
       <c r="B333" t="s">
         <v>645</v>
       </c>
-      <c r="C333" s="27">
+      <c r="C333" s="23">
         <v>1.0317783570102199</v>
       </c>
     </row>
@@ -28422,7 +28422,7 @@
       <c r="B334" t="s">
         <v>289</v>
       </c>
-      <c r="C334" s="27">
+      <c r="C334" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28433,7 +28433,7 @@
       <c r="B335" t="s">
         <v>289</v>
       </c>
-      <c r="C335" s="27">
+      <c r="C335" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28444,7 +28444,7 @@
       <c r="B336" t="s">
         <v>289</v>
       </c>
-      <c r="C336" s="27">
+      <c r="C336" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28455,7 +28455,7 @@
       <c r="B337" t="s">
         <v>289</v>
       </c>
-      <c r="C337" s="27">
+      <c r="C337" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28466,7 +28466,7 @@
       <c r="B338" t="s">
         <v>289</v>
       </c>
-      <c r="C338" s="27">
+      <c r="C338" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28477,7 +28477,7 @@
       <c r="B339" t="s">
         <v>289</v>
       </c>
-      <c r="C339" s="27">
+      <c r="C339" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28488,7 +28488,7 @@
       <c r="B340" t="s">
         <v>289</v>
       </c>
-      <c r="C340" s="27">
+      <c r="C340" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28499,7 +28499,7 @@
       <c r="B341" t="s">
         <v>289</v>
       </c>
-      <c r="C341" s="27">
+      <c r="C341" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28510,7 +28510,7 @@
       <c r="B342" t="s">
         <v>285</v>
       </c>
-      <c r="C342" s="27">
+      <c r="C342" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28521,7 +28521,7 @@
       <c r="B343" t="s">
         <v>285</v>
       </c>
-      <c r="C343" s="27">
+      <c r="C343" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28532,7 +28532,7 @@
       <c r="B344" t="s">
         <v>289</v>
       </c>
-      <c r="C344" s="27">
+      <c r="C344" s="23">
         <v>1.00141665435174</v>
       </c>
     </row>
@@ -28543,7 +28543,7 @@
       <c r="B345" t="s">
         <v>1478</v>
       </c>
-      <c r="C345" s="27">
+      <c r="C345" s="23">
         <v>0.40637195101645701</v>
       </c>
     </row>
@@ -28554,7 +28554,7 @@
       <c r="B346" t="s">
         <v>1483</v>
       </c>
-      <c r="C346" s="27">
+      <c r="C346" s="23">
         <v>0.40241649638941901</v>
       </c>
     </row>
@@ -28565,7 +28565,7 @@
       <c r="B347" t="s">
         <v>365</v>
       </c>
-      <c r="C347" s="27">
+      <c r="C347" s="23">
         <v>0.19741766022030499</v>
       </c>
     </row>
@@ -28576,7 +28576,7 @@
       <c r="B348" t="s">
         <v>369</v>
       </c>
-      <c r="C348" s="27">
+      <c r="C348" s="23">
         <v>0.19741766022030499</v>
       </c>
     </row>
@@ -28587,7 +28587,7 @@
       <c r="B349" t="s">
         <v>361</v>
       </c>
-      <c r="C349" s="27">
+      <c r="C349" s="23">
         <v>0.19741766022030499</v>
       </c>
     </row>
@@ -28598,7 +28598,7 @@
       <c r="B350" t="s">
         <v>388</v>
       </c>
-      <c r="C350" s="27">
+      <c r="C350" s="23">
         <v>9.9401734614570705E-2</v>
       </c>
     </row>
@@ -28609,7 +28609,7 @@
       <c r="B351" t="s">
         <v>388</v>
       </c>
-      <c r="C351" s="27">
+      <c r="C351" s="23">
         <v>9.9401734614570705E-2</v>
       </c>
     </row>
@@ -28620,7 +28620,7 @@
       <c r="B352" t="s">
         <v>1498</v>
       </c>
-      <c r="C352" s="26">
+      <c r="C352" s="22">
         <v>0</v>
       </c>
     </row>
@@ -28631,7 +28631,7 @@
       <c r="B353" t="s">
         <v>1498</v>
       </c>
-      <c r="C353" s="26">
+      <c r="C353" s="22">
         <v>0</v>
       </c>
     </row>
@@ -28642,7 +28642,7 @@
       <c r="B354" t="s">
         <v>1498</v>
       </c>
-      <c r="C354" s="26">
+      <c r="C354" s="22">
         <v>0</v>
       </c>
     </row>
@@ -28653,7 +28653,7 @@
       <c r="B355" t="s">
         <v>1498</v>
       </c>
-      <c r="C355" s="26">
+      <c r="C355" s="22">
         <v>0</v>
       </c>
     </row>
@@ -28664,7 +28664,7 @@
       <c r="B356" t="s">
         <v>1498</v>
       </c>
-      <c r="C356" s="26">
+      <c r="C356" s="22">
         <v>0</v>
       </c>
     </row>
@@ -28675,7 +28675,7 @@
       <c r="B357" t="s">
         <v>1498</v>
       </c>
-      <c r="C357" s="26">
+      <c r="C357" s="22">
         <v>0</v>
       </c>
     </row>
@@ -28686,7 +28686,7 @@
       <c r="B358" t="s">
         <v>1498</v>
       </c>
-      <c r="C358" s="26">
+      <c r="C358" s="22">
         <v>0</v>
       </c>
     </row>
@@ -28697,7 +28697,7 @@
       <c r="B359" t="s">
         <v>1498</v>
       </c>
-      <c r="C359" s="26">
+      <c r="C359" s="22">
         <v>0</v>
       </c>
     </row>
@@ -28708,7 +28708,7 @@
       <c r="B360" t="s">
         <v>1498</v>
       </c>
-      <c r="C360" s="26">
+      <c r="C360" s="22">
         <v>0</v>
       </c>
     </row>
@@ -28719,7 +28719,7 @@
       <c r="B361" t="s">
         <v>1498</v>
       </c>
-      <c r="C361" s="26">
+      <c r="C361" s="22">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reanalysis with new ecYali
</commit_message>
<xml_diff>
--- a/ecYaliGEM/output/enzymeUsage vs FSEOF.xlsx
+++ b/ecYaliGEM/output/enzymeUsage vs FSEOF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jujum\OneDrive\Documentos\GitHub\GECKO\ecYaliGEM\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F081B91F-2860-48AC-B43A-19AB753A3B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561626A0-5BF8-4544-926F-82F7A610E3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ecYali_Exp" sheetId="1" r:id="rId1"/>
@@ -5779,7 +5779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5817,14 +5817,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5885,17 +5883,6 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -5917,6 +5904,17 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -12544,7 +12542,7 @@
     <tableColumn id="7" xr3:uid="{B8AE34E5-96E2-4669-8C35-372E0E058E39}" name="Full capacity?" dataDxfId="17">
       <calculatedColumnFormula>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E29B3D2B-E0B4-4A3D-B4A6-3516D246A57F}" name="Coluna1" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{E29B3D2B-E0B4-4A3D-B4A6-3516D246A57F}" name="Coluna1" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12561,7 +12559,7 @@
   </autoFilter>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{376CAA50-40A1-4E7F-8703-DDDD2C53A76B}" name="Gene"/>
-    <tableColumn id="2" xr3:uid="{C96A8BC2-B7BA-4416-83AF-A6BE6C23B623}" name="K-score" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{C96A8BC2-B7BA-4416-83AF-A6BE6C23B623}" name="K-score" dataDxfId="15"/>
     <tableColumn id="3" xr3:uid="{28D3AAA4-C01E-4763-9813-BCBCDA6F710D}" name="rxnName"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -12596,7 +12594,7 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9828324B-B1A7-405F-BDF4-02AB298648CB}" name="rxnID"/>
     <tableColumn id="2" xr3:uid="{1D21A188-4E6E-4813-93C9-53303D94A8FA}" name="rxnName"/>
-    <tableColumn id="3" xr3:uid="{BD1DDBF5-5E6C-439F-AEE5-4B786B6139B8}" name="k-score (FSEOF)" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{BD1DDBF5-5E6C-439F-AEE5-4B786B6139B8}" name="k-score (FSEOF)" dataDxfId="14"/>
     <tableColumn id="4" xr3:uid="{69444D84-9159-4F7A-860D-B03514F4C1C6}" name="grRules"/>
     <tableColumn id="5" xr3:uid="{7FD0E090-AED0-437F-91AD-29933D0FD7AE}" name="rxnEquation"/>
     <tableColumn id="6" xr3:uid="{C1A1CBE8-80C2-47C9-8E2C-7ED9594B1DEC}" name="Full capacity?">
@@ -12614,14 +12612,14 @@
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{4905A0A7-9CA0-4B61-A17A-A60AA93CFAF9}" name="protID"/>
     <tableColumn id="2" xr3:uid="{07CE7141-993F-4265-ADA2-1D7AE02E2331}" name="geneID"/>
-    <tableColumn id="3" xr3:uid="{DD485713-254D-456F-A6A4-FF80A9F2504A}" name="absUsage" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{6ED1EEFA-F296-4FEE-8090-465370BDD4EB}" name="percUsage" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{8EF813D8-C987-4BEE-BB29-271B2A5ADA14}" name="kcat" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{DD485713-254D-456F-A6A4-FF80A9F2504A}" name="absUsage" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{6ED1EEFA-F296-4FEE-8090-465370BDD4EB}" name="percUsage" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{8EF813D8-C987-4BEE-BB29-271B2A5ADA14}" name="kcat" dataDxfId="11"/>
     <tableColumn id="6" xr3:uid="{E9482A6E-4578-462E-B118-408E2D0DD4F9}" name="sorce"/>
     <tableColumn id="7" xr3:uid="{3318B392-664A-4D18-A77D-DFA08B424AEA}" name="rxnID"/>
     <tableColumn id="8" xr3:uid="{54DDE929-E8C8-4736-9AD2-5FD58FCAE634}" name="rxnNames"/>
     <tableColumn id="9" xr3:uid="{44B3321F-81D2-4832-A9C4-ED4925AE4EEB}" name="grRules"/>
-    <tableColumn id="10" xr3:uid="{0A4F1D80-C65F-4E35-8820-A1CCE3DCC85B}" name="FSEOF?" dataDxfId="12">
+    <tableColumn id="10" xr3:uid="{0A4F1D80-C65F-4E35-8820-A1CCE3DCC85B}" name="FSEOF?" dataDxfId="10">
       <calculatedColumnFormula>COUNTIF(Tabela5[rxnID],G83)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{84091260-CE60-469A-9EF2-267494370C4C}" name="Full capacity?">
@@ -12660,7 +12658,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{87BE210B-E26E-4D99-9F75-2FB7BB547A2E}" name="Genes"/>
     <tableColumn id="2" xr3:uid="{9DB0997A-9630-447E-84DF-46C65C91CCBD}" name="Gene Names"/>
-    <tableColumn id="3" xr3:uid="{0E46B091-E495-4819-A523-84DE06CEF752}" name="k-scores" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{0E46B091-E495-4819-A523-84DE06CEF752}" name="k-scores" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12990,15 +12988,15 @@
       <c r="G1" s="26"/>
       <c r="H1" s="26"/>
       <c r="I1" s="26"/>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="27" t="s">
         <v>449</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -15220,7 +15218,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G74" s="29" t="s">
+      <c r="G74" t="s">
         <v>1539</v>
       </c>
       <c r="H74" s="8" t="s">
@@ -15256,7 +15254,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G75" s="29" t="s">
+      <c r="G75" t="s">
         <v>1542</v>
       </c>
       <c r="H75" s="4" t="s">
@@ -15292,7 +15290,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G76" s="29" t="s">
+      <c r="G76" t="s">
         <v>1546</v>
       </c>
       <c r="H76" s="5" t="s">
@@ -15328,7 +15326,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G77" s="29" t="s">
+      <c r="G77" t="s">
         <v>1549</v>
       </c>
       <c r="J77" t="s">
@@ -15361,7 +15359,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G78" s="29" t="s">
+      <c r="G78" t="s">
         <v>1539</v>
       </c>
       <c r="J78" t="s">
@@ -15394,7 +15392,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G79" s="29" t="s">
+      <c r="G79" t="s">
         <v>1554</v>
       </c>
       <c r="J79" t="s">
@@ -15427,7 +15425,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G80" s="29" t="s">
+      <c r="G80" t="s">
         <v>1558</v>
       </c>
       <c r="J80" t="s">
@@ -15460,7 +15458,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G81" s="29" t="s">
+      <c r="G81" t="s">
         <v>1562</v>
       </c>
       <c r="J81" t="s">
@@ -15493,7 +15491,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G82" s="29" t="s">
+      <c r="G82" t="s">
         <v>1566</v>
       </c>
       <c r="J82" t="s">
@@ -15526,7 +15524,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G83" s="29" t="s">
+      <c r="G83" t="s">
         <v>1566</v>
       </c>
       <c r="J83" t="s">
@@ -15559,7 +15557,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G84" s="29" t="s">
+      <c r="G84" t="s">
         <v>1570</v>
       </c>
       <c r="J84" t="s">
@@ -15592,7 +15590,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G85" s="29" t="s">
+      <c r="G85" t="s">
         <v>269</v>
       </c>
       <c r="J85" t="s">
@@ -15625,7 +15623,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G86" s="29" t="s">
+      <c r="G86" t="s">
         <v>238</v>
       </c>
       <c r="J86" t="s">
@@ -15658,7 +15656,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G87" s="29" t="s">
+      <c r="G87" t="s">
         <v>265</v>
       </c>
       <c r="J87" t="s">
@@ -15691,7 +15689,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G88" s="29" t="s">
+      <c r="G88" t="s">
         <v>1576</v>
       </c>
       <c r="J88" t="s">
@@ -15724,7 +15722,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G89" s="29" t="s">
+      <c r="G89" t="s">
         <v>250</v>
       </c>
       <c r="J89" t="s">
@@ -15757,7 +15755,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G90" s="29" t="s">
+      <c r="G90" t="s">
         <v>262</v>
       </c>
       <c r="J90" t="s">
@@ -15790,7 +15788,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G91" s="29" t="s">
+      <c r="G91" t="s">
         <v>273</v>
       </c>
       <c r="J91" t="s">
@@ -15823,7 +15821,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G92" s="29" t="s">
+      <c r="G92" t="s">
         <v>1581</v>
       </c>
       <c r="J92" t="s">
@@ -15856,7 +15854,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G93" s="29" t="s">
+      <c r="G93" t="s">
         <v>1585</v>
       </c>
       <c r="J93" t="s">
@@ -15889,7 +15887,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G94" s="29" t="s">
+      <c r="G94" t="s">
         <v>1588</v>
       </c>
       <c r="J94" t="s">
@@ -15922,7 +15920,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G95" s="29" t="s">
+      <c r="G95" t="s">
         <v>1592</v>
       </c>
       <c r="J95" t="s">
@@ -15955,7 +15953,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G96" s="29" t="s">
+      <c r="G96" t="s">
         <v>1594</v>
       </c>
       <c r="J96" t="s">
@@ -15988,7 +15986,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G97" s="29" t="s">
+      <c r="G97" t="s">
         <v>1596</v>
       </c>
       <c r="J97" t="s">
@@ -16021,7 +16019,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G98" s="29" t="s">
+      <c r="G98" t="s">
         <v>1598</v>
       </c>
       <c r="J98" t="s">
@@ -16054,7 +16052,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G99" s="29" t="s">
+      <c r="G99" t="s">
         <v>1600</v>
       </c>
       <c r="J99" t="s">
@@ -16087,7 +16085,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G100" s="29" t="s">
+      <c r="G100" t="s">
         <v>1602</v>
       </c>
       <c r="J100" t="s">
@@ -16120,7 +16118,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G101" s="29" t="s">
+      <c r="G101" t="s">
         <v>1604</v>
       </c>
       <c r="J101" t="s">
@@ -16150,7 +16148,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G102" s="29" t="s">
+      <c r="G102" t="s">
         <v>1606</v>
       </c>
       <c r="J102" t="s">
@@ -16180,7 +16178,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>1</v>
       </c>
-      <c r="G103" s="29" t="s">
+      <c r="G103" t="s">
         <v>1461</v>
       </c>
       <c r="J103" t="s">
@@ -16210,7 +16208,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G104" s="29" t="s">
+      <c r="G104" t="s">
         <v>1609</v>
       </c>
       <c r="J104" t="s">
@@ -16240,7 +16238,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G105" s="29" t="s">
+      <c r="G105" t="s">
         <v>1612</v>
       </c>
       <c r="J105" t="s">
@@ -16273,7 +16271,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G106" s="29" t="s">
+      <c r="G106" t="s">
         <v>1614</v>
       </c>
       <c r="J106" t="s">
@@ -16303,7 +16301,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G107" s="29" t="s">
+      <c r="G107" t="s">
         <v>1617</v>
       </c>
       <c r="J107" t="s">
@@ -16333,7 +16331,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G108" s="29" t="s">
+      <c r="G108" t="s">
         <v>1621</v>
       </c>
       <c r="J108" t="s">
@@ -16366,7 +16364,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>2</v>
       </c>
-      <c r="G109" s="29" t="s">
+      <c r="G109" t="s">
         <v>1474</v>
       </c>
       <c r="J109" t="s">
@@ -16399,7 +16397,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G110" s="29" t="s">
+      <c r="G110" t="s">
         <v>1628</v>
       </c>
       <c r="J110" t="s">
@@ -16429,7 +16427,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G111" s="29" t="s">
+      <c r="G111" t="s">
         <v>1632</v>
       </c>
       <c r="J111" t="s">
@@ -16462,7 +16460,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G112" s="29" t="s">
+      <c r="G112" t="s">
         <v>1542</v>
       </c>
       <c r="J112" t="s">
@@ -16492,7 +16490,7 @@
         <f>COUNTIF(Tabela1[rxnName],Tabela2[[#This Row],[rxnName]])</f>
         <v>0</v>
       </c>
-      <c r="G113" s="29" t="s">
+      <c r="G113" t="s">
         <v>227</v>
       </c>
       <c r="J113" t="s">
@@ -16522,7 +16520,7 @@
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G114" s="29" t="s">
+      <c r="G114" t="s">
         <v>1640</v>
       </c>
       <c r="J114" t="s">
@@ -16552,7 +16550,7 @@
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G115" s="29" t="s">
+      <c r="G115" t="s">
         <v>1643</v>
       </c>
       <c r="J115" t="s">
@@ -16582,7 +16580,7 @@
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G116" s="29" t="s">
+      <c r="G116" t="s">
         <v>1474</v>
       </c>
       <c r="J116" t="s">
@@ -16612,7 +16610,7 @@
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G117" s="29" t="s">
+      <c r="G117" t="s">
         <v>1648</v>
       </c>
       <c r="J117" t="s">
@@ -16642,7 +16640,7 @@
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G118" s="29" t="s">
+      <c r="G118" t="s">
         <v>1648</v>
       </c>
       <c r="J118" t="s">
@@ -16675,7 +16673,7 @@
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G119" s="29" t="s">
+      <c r="G119" t="s">
         <v>1654</v>
       </c>
       <c r="J119" t="s">
@@ -16705,7 +16703,7 @@
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G120" s="29" t="s">
+      <c r="G120" t="s">
         <v>1493</v>
       </c>
       <c r="J120" t="s">
@@ -16735,7 +16733,7 @@
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G121" s="29" t="s">
+      <c r="G121" t="s">
         <v>1497</v>
       </c>
       <c r="J121" t="s">
@@ -16765,7 +16763,7 @@
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G122" s="29" t="s">
+      <c r="G122" t="s">
         <v>1501</v>
       </c>
     </row>
@@ -16789,127 +16787,127 @@
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G123" s="29" t="s">
+      <c r="G123" t="s">
         <v>1663</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A124" s="29" t="s">
+      <c r="A124" t="s">
         <v>1666</v>
       </c>
-      <c r="B124" s="29" t="s">
+      <c r="B124" t="s">
         <v>1667</v>
       </c>
-      <c r="C124" s="30">
-        <v>0</v>
-      </c>
-      <c r="D124" s="29" t="s">
+      <c r="C124" s="16">
+        <v>0</v>
+      </c>
+      <c r="D124" t="s">
         <v>1664</v>
       </c>
-      <c r="E124" s="29" t="s">
+      <c r="E124" t="s">
         <v>1668</v>
       </c>
-      <c r="F124" s="29">
+      <c r="F124">
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G124" s="29" t="s">
+      <c r="G124" t="s">
         <v>1667</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A125" s="29" t="s">
+      <c r="A125" t="s">
         <v>1172</v>
       </c>
-      <c r="B125" s="29" t="s">
+      <c r="B125" t="s">
         <v>1669</v>
       </c>
-      <c r="C125" s="30">
-        <v>0</v>
-      </c>
-      <c r="D125" s="29" t="s">
+      <c r="C125" s="16">
+        <v>0</v>
+      </c>
+      <c r="D125" t="s">
         <v>1670</v>
       </c>
-      <c r="E125" s="29" t="s">
+      <c r="E125" t="s">
         <v>1671</v>
       </c>
-      <c r="F125" s="29">
+      <c r="F125">
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G125" s="29" t="s">
+      <c r="G125" t="s">
         <v>1669</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A126" s="29" t="s">
+      <c r="A126" t="s">
         <v>1672</v>
       </c>
-      <c r="B126" s="29" t="s">
+      <c r="B126" t="s">
         <v>1673</v>
       </c>
-      <c r="C126" s="30">
-        <v>0</v>
-      </c>
-      <c r="D126" s="29" t="s">
+      <c r="C126" s="16">
+        <v>0</v>
+      </c>
+      <c r="D126" t="s">
         <v>1674</v>
       </c>
-      <c r="E126" s="29" t="s">
+      <c r="E126" t="s">
         <v>1675</v>
       </c>
-      <c r="F126" s="29">
+      <c r="F126">
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G126" s="29" t="s">
+      <c r="G126" t="s">
         <v>1673</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A127" s="29" t="s">
+      <c r="A127" t="s">
         <v>1398</v>
       </c>
-      <c r="B127" s="29" t="s">
+      <c r="B127" t="s">
         <v>1676</v>
       </c>
-      <c r="C127" s="30">
-        <v>0</v>
-      </c>
-      <c r="D127" s="29" t="s">
+      <c r="C127" s="16">
+        <v>0</v>
+      </c>
+      <c r="D127" t="s">
         <v>1677</v>
       </c>
-      <c r="E127" s="29" t="s">
+      <c r="E127" t="s">
         <v>1678</v>
       </c>
-      <c r="F127" s="29">
+      <c r="F127">
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G127" s="29" t="s">
+      <c r="G127" t="s">
         <v>1676</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A128" s="29" t="s">
+      <c r="A128" t="s">
         <v>1196</v>
       </c>
-      <c r="B128" s="29" t="s">
+      <c r="B128" t="s">
         <v>1679</v>
       </c>
-      <c r="C128" s="30">
-        <v>0</v>
-      </c>
-      <c r="D128" s="29" t="s">
+      <c r="C128" s="16">
+        <v>0</v>
+      </c>
+      <c r="D128" t="s">
         <v>1680</v>
       </c>
-      <c r="E128" s="29" t="s">
+      <c r="E128" t="s">
         <v>1681</v>
       </c>
-      <c r="F128" s="29">
+      <c r="F128">
         <f>COUNTIF(Tabela1[rxnID],Tabela2[[#This Row],[rxnID]])</f>
         <v>0</v>
       </c>
-      <c r="G128" s="29" t="s">
+      <c r="G128" t="s">
         <v>1679</v>
       </c>
     </row>
@@ -17083,7 +17081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD147150-DDDE-4176-9567-786D2C29D3F7}">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A83" sqref="A83:H105"/>
     </sheetView>
   </sheetViews>
@@ -17141,15 +17139,15 @@
       <c r="H2" t="s">
         <v>176</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="27" t="s">
         <v>459</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -19170,19 +19168,19 @@
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A81" s="27" t="s">
+      <c r="A81" s="28" t="s">
         <v>404</v>
       </c>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27"/>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="27"/>
-      <c r="H81" s="27"/>
-      <c r="I81" s="27"/>
-      <c r="J81" s="27"/>
-      <c r="K81" s="27"/>
+      <c r="B81" s="28"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="28"/>
+      <c r="G81" s="28"/>
+      <c r="H81" s="28"/>
+      <c r="I81" s="28"/>
+      <c r="J81" s="28"/>
+      <c r="K81" s="28"/>
       <c r="M81" t="s">
         <v>275</v>
       </c>
@@ -20204,7 +20202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EFCAA3-E27B-4FE4-B624-75200D03C114}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FSEOF with tighter range
</commit_message>
<xml_diff>
--- a/ecYaliGEM/output/enzymeUsage vs FSEOF.xlsx
+++ b/ecYaliGEM/output/enzymeUsage vs FSEOF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jusabe\Documents\GECKO\ecYaliGEM\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADADFDA1-5F00-4DED-A664-01C0408FB722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE7A5E5-BFFC-4DD9-81E6-1F92FF33AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="2520" windowWidth="14400" windowHeight="15600" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ecYali_Exp" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4397" uniqueCount="2458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4405" uniqueCount="2465">
   <si>
     <t>'YALI0E02728g'</t>
   </si>
@@ -7412,10 +7412,31 @@
     <t>'''ATP[c] + citrate[c] + coenzyme A[c] + 0.33814 prot_Q6C3H5[c] + 0.25611 prot_Q6C7Y1[c] =&gt; acetyl-CoA[c] + ADP[c] + oxaloacetate[c...'' &lt;Preview truncated at 128 characters&gt;'</t>
   </si>
   <si>
-    <t>(S)-malate[m] + NAD[m] + 0.14314 prot_Q6C5F0[c] =&gt; carbon dioxide[m] + NADH[m] + pyruvate[m]'</t>
-  </si>
-  <si>
-    <t>H2O[c] + L-glutamate[c] + NAD[c] + 0.23878 prot_Q6C6H1[c] =&gt; 2-oxoglutarate[c] + ammonium[c] + H+[c] + NADH[c]'</t>
+    <t>'(S)-malate[m] + NAD[m] + 0.14314 prot_Q6C5F0[c] =&gt; carbon dioxide[m] + NADH[m] + pyruvate[m]'</t>
+  </si>
+  <si>
+    <t>'H2O[c] + L-glutamate[c] + NAD[c] + 0.23878 prot_Q6C6H1[c] =&gt; 2-oxoglutarate[c] + ammonium[c] + H+[c] + NADH[c]'</t>
+  </si>
+  <si>
+    <t>'y102884'</t>
+  </si>
+  <si>
+    <t>'PE diacylglycerol acyltransferase'</t>
+  </si>
+  <si>
+    <t>'''diglyceride[erm] + phosphatidylethanolamine[erm] + 0.51315 prot_Q6C5M4[c] =&gt; 1-acylglycerophosphoethanolamine[erm] + triglycerid...'' &lt;Preview truncated at 128 characters&gt;'</t>
+  </si>
+  <si>
+    <t>'y103312'</t>
+  </si>
+  <si>
+    <t>'lysoPE acyltransferase, lipid particle'</t>
+  </si>
+  <si>
+    <t>'YALI0D16379g'</t>
+  </si>
+  <si>
+    <t>'1-acylglycerophosphoethanolamine[lp] + acyl-CoA[lp] + 0.001666 prot_Q6C8W4[c] =&gt; phosphatidylethanolamine[lp] + coenzyme A[lp]'</t>
   </si>
 </sst>
 </file>
@@ -7522,7 +7543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -7570,14 +7591,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="34">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -7633,6 +7652,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -14445,15 +14467,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7F0AA8EA-476C-4F4B-80F4-DE8A34E64E46}" name="Tabela5" displayName="Tabela5" ref="L35:R80" totalsRowShown="0">
-  <autoFilter ref="L35:R80" xr:uid="{7F0AA8EA-476C-4F4B-80F4-DE8A34E64E46}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7F0AA8EA-476C-4F4B-80F4-DE8A34E64E46}" name="Tabela5" displayName="Tabela5" ref="L35:R82" totalsRowShown="0">
+  <autoFilter ref="L35:R82" xr:uid="{7F0AA8EA-476C-4F4B-80F4-DE8A34E64E46}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9828324B-B1A7-405F-BDF4-02AB298648CB}" name="rxnID"/>
     <tableColumn id="2" xr3:uid="{1D21A188-4E6E-4813-93C9-53303D94A8FA}" name="rxnName"/>
     <tableColumn id="3" xr3:uid="{BD1DDBF5-5E6C-439F-AEE5-4B786B6139B8}" name="k-score (FSEOF)" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{69444D84-9159-4F7A-860D-B03514F4C1C6}" name="grRules"/>
     <tableColumn id="5" xr3:uid="{7FD0E090-AED0-437F-91AD-29933D0FD7AE}" name="rxnEquation"/>
-    <tableColumn id="6" xr3:uid="{C1A1CBE8-80C2-47C9-8E2C-7ED9594B1DEC}" name="Full capacity?" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{C1A1CBE8-80C2-47C9-8E2C-7ED9594B1DEC}" name="Full capacity?" dataDxfId="11">
       <calculatedColumnFormula>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{E511D38C-DB49-458B-B4DE-F2D62D623BAD}" name="Comments"/>
@@ -14468,14 +14490,14 @@
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{4905A0A7-9CA0-4B61-A17A-A60AA93CFAF9}" name="protID"/>
     <tableColumn id="2" xr3:uid="{07CE7141-993F-4265-ADA2-1D7AE02E2331}" name="geneID"/>
-    <tableColumn id="3" xr3:uid="{DD485713-254D-456F-A6A4-FF80A9F2504A}" name="absUsage" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{6ED1EEFA-F296-4FEE-8090-465370BDD4EB}" name="percUsage" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{8EF813D8-C987-4BEE-BB29-271B2A5ADA14}" name="kcat" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{DD485713-254D-456F-A6A4-FF80A9F2504A}" name="absUsage" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{6ED1EEFA-F296-4FEE-8090-465370BDD4EB}" name="percUsage" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{8EF813D8-C987-4BEE-BB29-271B2A5ADA14}" name="kcat" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{E9482A6E-4578-462E-B118-408E2D0DD4F9}" name="sorce"/>
     <tableColumn id="7" xr3:uid="{3318B392-664A-4D18-A77D-DFA08B424AEA}" name="rxnID"/>
     <tableColumn id="8" xr3:uid="{54DDE929-E8C8-4736-9AD2-5FD58FCAE634}" name="rxnNames"/>
     <tableColumn id="9" xr3:uid="{44B3321F-81D2-4832-A9C4-ED4925AE4EEB}" name="grRules"/>
-    <tableColumn id="10" xr3:uid="{0A4F1D80-C65F-4E35-8820-A1CCE3DCC85B}" name="FSEOF?" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{0A4F1D80-C65F-4E35-8820-A1CCE3DCC85B}" name="FSEOF?" dataDxfId="7">
       <calculatedColumnFormula>COUNTIF(Tabela5[rxnID],R94)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{84091260-CE60-469A-9EF2-267494370C4C}" name="Full capacity?">
@@ -14514,7 +14536,7 @@
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{87BE210B-E26E-4D99-9F75-2FB7BB547A2E}" name="Genes"/>
     <tableColumn id="2" xr3:uid="{9DB0997A-9630-447E-84DF-46C65C91CCBD}" name="Gene Names"/>
-    <tableColumn id="3" xr3:uid="{0E46B091-E495-4819-A523-84DE06CEF752}" name="k-scores" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0E46B091-E495-4819-A523-84DE06CEF752}" name="k-scores" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18902,24 +18924,24 @@
     <mergeCell ref="K1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="C74:C113">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>C74&lt;0.5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>C74&lt;0.05</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>C74&gt;=1.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K74:K121">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>K74&lt;0.5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>K74&lt;0.05</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>K74&gt;=1.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18937,8 +18959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD147150-DDDE-4176-9567-786D2C29D3F7}">
   <dimension ref="A1:V359"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView topLeftCell="L31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N77" sqref="N77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18956,6 +18978,7 @@
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
     <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="71" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="52.42578125" customWidth="1"/>
     <col min="16" max="16" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -20025,7 +20048,7 @@
         <v>484</v>
       </c>
       <c r="N36">
-        <v>7.0188994892474099</v>
+        <v>7.2380793002505603</v>
       </c>
       <c r="O36" t="s">
         <v>485</v>
@@ -20068,7 +20091,7 @@
         <v>1064</v>
       </c>
       <c r="N37">
-        <v>2.6841952033690002</v>
+        <v>2.7045251959609899</v>
       </c>
       <c r="O37" t="s">
         <v>474</v>
@@ -20111,7 +20134,7 @@
         <v>2365</v>
       </c>
       <c r="N38">
-        <v>2.4484005684457899</v>
+        <v>2.3748145435805901</v>
       </c>
       <c r="O38" t="s">
         <v>2366</v>
@@ -20148,19 +20171,19 @@
       </c>
       <c r="H39" s="24"/>
       <c r="L39" t="s">
-        <v>2367</v>
+        <v>2458</v>
       </c>
       <c r="M39" t="s">
-        <v>100</v>
+        <v>2459</v>
       </c>
       <c r="N39">
-        <v>1.2190082359602701</v>
+        <v>1.544309023012</v>
       </c>
       <c r="O39" t="s">
-        <v>101</v>
+        <v>379</v>
       </c>
       <c r="P39" t="s">
-        <v>2368</v>
+        <v>2460</v>
       </c>
       <c r="Q39">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20191,19 +20214,19 @@
       </c>
       <c r="H40" s="24"/>
       <c r="L40" t="s">
-        <v>2369</v>
+        <v>2461</v>
       </c>
       <c r="M40" t="s">
-        <v>92</v>
+        <v>2462</v>
       </c>
       <c r="N40">
-        <v>1.17585824591855</v>
+        <v>1.544309023012</v>
       </c>
       <c r="O40" t="s">
-        <v>93</v>
+        <v>2463</v>
       </c>
       <c r="P40" t="s">
-        <v>2370</v>
+        <v>2464</v>
       </c>
       <c r="Q40">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20234,23 +20257,23 @@
       </c>
       <c r="H41" s="24"/>
       <c r="L41" t="s">
-        <v>1824</v>
+        <v>2367</v>
       </c>
       <c r="M41" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="N41">
-        <v>1.17585824591855</v>
+        <v>1.2095971735256099</v>
       </c>
       <c r="O41" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="P41" t="s">
-        <v>2371</v>
+        <v>2368</v>
       </c>
       <c r="Q41">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -20277,19 +20300,19 @@
       </c>
       <c r="H42" s="24"/>
       <c r="L42" t="s">
-        <v>2372</v>
+        <v>2369</v>
       </c>
       <c r="M42" t="s">
-        <v>1052</v>
+        <v>92</v>
       </c>
       <c r="N42">
-        <v>1.1609242185147699</v>
+        <v>1.1684407503059</v>
       </c>
       <c r="O42" t="s">
-        <v>1053</v>
+        <v>93</v>
       </c>
       <c r="P42" t="s">
-        <v>2373</v>
+        <v>2370</v>
       </c>
       <c r="Q42">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20320,23 +20343,23 @@
       </c>
       <c r="H43" s="24"/>
       <c r="L43" t="s">
-        <v>2374</v>
+        <v>1824</v>
       </c>
       <c r="M43" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="N43">
-        <v>1.0997909299940201</v>
+        <v>1.1684407503059</v>
       </c>
       <c r="O43" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="P43" t="s">
-        <v>2375</v>
+        <v>2371</v>
       </c>
       <c r="Q43">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -20363,19 +20386,19 @@
       </c>
       <c r="H44" s="24"/>
       <c r="L44" t="s">
-        <v>2376</v>
+        <v>2372</v>
       </c>
       <c r="M44" t="s">
-        <v>104</v>
+        <v>1052</v>
       </c>
       <c r="N44">
-        <v>1.0997909299940201</v>
+        <v>1.1499895487564</v>
       </c>
       <c r="O44" t="s">
-        <v>105</v>
+        <v>1053</v>
       </c>
       <c r="P44" t="s">
-        <v>2377</v>
+        <v>2373</v>
       </c>
       <c r="Q44">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20406,19 +20429,19 @@
       </c>
       <c r="H45" s="24"/>
       <c r="L45" t="s">
-        <v>2378</v>
+        <v>2374</v>
       </c>
       <c r="M45" t="s">
-        <v>352</v>
+        <v>102</v>
       </c>
       <c r="N45">
-        <v>1.0381358142406401</v>
+        <v>1.09494022622396</v>
       </c>
       <c r="O45" t="s">
-        <v>353</v>
+        <v>103</v>
       </c>
       <c r="P45" t="s">
-        <v>2379</v>
+        <v>2375</v>
       </c>
       <c r="Q45">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20449,19 +20472,19 @@
       </c>
       <c r="H46" s="24"/>
       <c r="L46" t="s">
-        <v>2388</v>
+        <v>2376</v>
       </c>
       <c r="M46" t="s">
-        <v>1020</v>
+        <v>104</v>
       </c>
       <c r="N46">
-        <v>0.631752195053499</v>
+        <v>1.09494022622396</v>
       </c>
       <c r="O46" t="s">
-        <v>882</v>
+        <v>105</v>
       </c>
       <c r="P46" t="s">
-        <v>2389</v>
+        <v>2377</v>
       </c>
       <c r="Q46">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20492,23 +20515,23 @@
       </c>
       <c r="H47" s="24"/>
       <c r="L47" t="s">
-        <v>1996</v>
+        <v>2378</v>
       </c>
       <c r="M47" t="s">
-        <v>1007</v>
+        <v>352</v>
       </c>
       <c r="N47">
-        <v>0.631752195051968</v>
+        <v>1.0362584560685799</v>
       </c>
       <c r="O47" t="s">
-        <v>870</v>
+        <v>353</v>
       </c>
       <c r="P47" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="Q47">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -20535,19 +20558,19 @@
       </c>
       <c r="H48" s="24"/>
       <c r="L48" t="s">
-        <v>2381</v>
+        <v>2388</v>
       </c>
       <c r="M48" t="s">
-        <v>2040</v>
+        <v>1020</v>
       </c>
       <c r="N48">
-        <v>0.631752195051968</v>
+        <v>0.64947286910628599</v>
       </c>
       <c r="O48" t="s">
-        <v>2382</v>
+        <v>882</v>
       </c>
       <c r="P48" t="s">
-        <v>2383</v>
+        <v>2389</v>
       </c>
       <c r="Q48">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20578,23 +20601,23 @@
       </c>
       <c r="H49" s="24"/>
       <c r="L49" t="s">
-        <v>2384</v>
+        <v>1996</v>
       </c>
       <c r="M49" t="s">
-        <v>1901</v>
+        <v>1007</v>
       </c>
       <c r="N49">
-        <v>0.631752195051968</v>
+        <v>0.64947286910262003</v>
       </c>
       <c r="O49" t="s">
-        <v>2382</v>
+        <v>870</v>
       </c>
       <c r="P49" t="s">
-        <v>2385</v>
+        <v>2380</v>
       </c>
       <c r="Q49">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -20621,19 +20644,19 @@
       </c>
       <c r="H50" s="24"/>
       <c r="L50" t="s">
-        <v>2386</v>
+        <v>2381</v>
       </c>
       <c r="M50" t="s">
-        <v>881</v>
+        <v>2040</v>
       </c>
       <c r="N50">
-        <v>0.631752195051968</v>
+        <v>0.64947286910261903</v>
       </c>
       <c r="O50" t="s">
-        <v>882</v>
+        <v>2382</v>
       </c>
       <c r="P50" t="s">
-        <v>2387</v>
+        <v>2383</v>
       </c>
       <c r="Q50">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20664,19 +20687,19 @@
       </c>
       <c r="H51" s="24"/>
       <c r="L51" t="s">
-        <v>2390</v>
+        <v>2386</v>
       </c>
       <c r="M51" t="s">
-        <v>85</v>
+        <v>881</v>
       </c>
       <c r="N51">
-        <v>0.63175219503435198</v>
+        <v>0.64947286910261903</v>
       </c>
       <c r="O51" t="s">
-        <v>86</v>
+        <v>882</v>
       </c>
       <c r="P51" t="s">
-        <v>2391</v>
+        <v>2387</v>
       </c>
       <c r="Q51">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20707,19 +20730,19 @@
       </c>
       <c r="H52" s="24"/>
       <c r="L52" t="s">
-        <v>2392</v>
+        <v>2384</v>
       </c>
       <c r="M52" t="s">
-        <v>120</v>
+        <v>1901</v>
       </c>
       <c r="N52">
-        <v>0.52206429407742405</v>
+        <v>0.64947286910261903</v>
       </c>
       <c r="O52" t="s">
-        <v>121</v>
+        <v>2382</v>
       </c>
       <c r="P52" t="s">
-        <v>2393</v>
+        <v>2385</v>
       </c>
       <c r="Q52">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20750,19 +20773,19 @@
       </c>
       <c r="H53" s="24"/>
       <c r="L53" t="s">
-        <v>2394</v>
+        <v>2390</v>
       </c>
       <c r="M53" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="N53">
-        <v>0.52206429407742405</v>
+        <v>0.64947286908278701</v>
       </c>
       <c r="O53" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="P53" t="s">
-        <v>2395</v>
+        <v>2391</v>
       </c>
       <c r="Q53">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20793,23 +20816,23 @@
       </c>
       <c r="H54" s="24"/>
       <c r="L54" t="s">
-        <v>1972</v>
+        <v>2392</v>
       </c>
       <c r="M54" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N54">
-        <v>0.52206429407742405</v>
+        <v>0.53670821816813297</v>
       </c>
       <c r="O54" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="P54" t="s">
-        <v>2396</v>
+        <v>2393</v>
       </c>
       <c r="Q54">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:17">
@@ -20836,19 +20859,19 @@
       </c>
       <c r="H55" s="24"/>
       <c r="L55" t="s">
-        <v>2397</v>
+        <v>2394</v>
       </c>
       <c r="M55" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="N55">
-        <v>0.44531351606153602</v>
+        <v>0.53670821816813297</v>
       </c>
       <c r="O55" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
       <c r="P55" t="s">
-        <v>2398</v>
+        <v>2395</v>
       </c>
       <c r="Q55">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -20879,23 +20902,23 @@
       </c>
       <c r="H56" s="24"/>
       <c r="L56" t="s">
-        <v>2399</v>
+        <v>1972</v>
       </c>
       <c r="M56" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="N56">
-        <v>0.44531351606153602</v>
+        <v>0.53670821816813297</v>
       </c>
       <c r="O56" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="P56" t="s">
-        <v>2400</v>
+        <v>2396</v>
       </c>
       <c r="Q56">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:17">
@@ -20922,23 +20945,23 @@
       </c>
       <c r="H57" s="24"/>
       <c r="L57" t="s">
-        <v>1754</v>
+        <v>2397</v>
       </c>
       <c r="M57" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
       <c r="N57">
-        <v>0.31605242286212099</v>
+        <v>0.456738807061629</v>
       </c>
       <c r="O57" t="s">
-        <v>1756</v>
+        <v>172</v>
       </c>
       <c r="P57" t="s">
-        <v>2401</v>
+        <v>2398</v>
       </c>
       <c r="Q57">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:17">
@@ -20965,19 +20988,19 @@
       </c>
       <c r="H58" s="24"/>
       <c r="L58" t="s">
-        <v>2402</v>
+        <v>2399</v>
       </c>
       <c r="M58" t="s">
-        <v>1036</v>
+        <v>173</v>
       </c>
       <c r="N58">
-        <v>0.31338233886130501</v>
+        <v>0.456738807061629</v>
       </c>
       <c r="O58" t="s">
-        <v>882</v>
+        <v>174</v>
       </c>
       <c r="P58" t="s">
-        <v>2403</v>
+        <v>2400</v>
       </c>
       <c r="Q58">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21008,23 +21031,23 @@
       </c>
       <c r="H59" s="24"/>
       <c r="L59" t="s">
-        <v>2404</v>
+        <v>1754</v>
       </c>
       <c r="M59" t="s">
-        <v>2405</v>
+        <v>131</v>
       </c>
       <c r="N59">
-        <v>0.28868017968772403</v>
+        <v>0.324917705819664</v>
       </c>
       <c r="O59" t="s">
-        <v>2406</v>
+        <v>1756</v>
       </c>
       <c r="P59" t="s">
-        <v>2407</v>
+        <v>2401</v>
       </c>
       <c r="Q59">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -21051,23 +21074,23 @@
       </c>
       <c r="H60" s="24"/>
       <c r="L60" t="s">
-        <v>2076</v>
+        <v>2402</v>
       </c>
       <c r="M60" t="s">
-        <v>1047</v>
+        <v>1036</v>
       </c>
       <c r="N60">
-        <v>0.26264247165557902</v>
+        <v>0.32217272585748402</v>
       </c>
       <c r="O60" t="s">
-        <v>1048</v>
+        <v>882</v>
       </c>
       <c r="P60" t="s">
-        <v>2409</v>
+        <v>2403</v>
       </c>
       <c r="Q60">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -21094,19 +21117,19 @@
       </c>
       <c r="H61" s="24"/>
       <c r="L61" t="s">
-        <v>2410</v>
+        <v>2404</v>
       </c>
       <c r="M61" t="s">
-        <v>2036</v>
+        <v>2405</v>
       </c>
       <c r="N61">
-        <v>0.23483084697831699</v>
+        <v>0.29676466281498898</v>
       </c>
       <c r="O61" t="s">
-        <v>2382</v>
+        <v>2406</v>
       </c>
       <c r="P61" t="s">
-        <v>2411</v>
+        <v>2407</v>
       </c>
       <c r="Q61">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21137,23 +21160,23 @@
       </c>
       <c r="H62" s="24"/>
       <c r="L62" t="s">
-        <v>2412</v>
+        <v>2076</v>
       </c>
       <c r="M62" t="s">
-        <v>19</v>
+        <v>1047</v>
       </c>
       <c r="N62">
-        <v>0.20677177330187599</v>
+        <v>0.27000960336962498</v>
       </c>
       <c r="O62" t="s">
-        <v>2413</v>
+        <v>1048</v>
       </c>
       <c r="P62" t="s">
-        <v>2414</v>
+        <v>2409</v>
       </c>
       <c r="Q62">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:17">
@@ -21180,23 +21203,23 @@
       </c>
       <c r="H63" s="24"/>
       <c r="L63" t="s">
-        <v>2015</v>
+        <v>2410</v>
       </c>
       <c r="M63" t="s">
-        <v>42</v>
+        <v>2036</v>
       </c>
       <c r="N63">
-        <v>0.18960092532175099</v>
+        <v>0.24141786152125599</v>
       </c>
       <c r="O63" t="s">
-        <v>2009</v>
+        <v>2382</v>
       </c>
       <c r="P63" t="s">
-        <v>2408</v>
+        <v>2411</v>
       </c>
       <c r="Q63">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:17">
@@ -21223,19 +21246,19 @@
       </c>
       <c r="H64" s="24"/>
       <c r="L64" t="s">
-        <v>2416</v>
+        <v>2412</v>
       </c>
       <c r="M64" t="s">
-        <v>2417</v>
+        <v>19</v>
       </c>
       <c r="N64">
-        <v>0.116662194772553</v>
+        <v>0.212555616893951</v>
       </c>
       <c r="O64" t="s">
-        <v>2418</v>
+        <v>2413</v>
       </c>
       <c r="P64" t="s">
-        <v>2419</v>
+        <v>2414</v>
       </c>
       <c r="Q64">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21266,23 +21289,23 @@
       </c>
       <c r="H65" s="24"/>
       <c r="L65" t="s">
-        <v>2420</v>
+        <v>2015</v>
       </c>
       <c r="M65" t="s">
-        <v>953</v>
+        <v>42</v>
       </c>
       <c r="N65">
-        <v>0.111325207686039</v>
+        <v>0.194919238773437</v>
       </c>
       <c r="O65" t="s">
-        <v>464</v>
+        <v>2009</v>
       </c>
       <c r="P65" t="s">
-        <v>2421</v>
+        <v>2408</v>
       </c>
       <c r="Q65">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:17">
@@ -21309,19 +21332,19 @@
       </c>
       <c r="H66" s="24"/>
       <c r="L66" t="s">
-        <v>2422</v>
+        <v>2416</v>
       </c>
       <c r="M66" t="s">
-        <v>108</v>
+        <v>2417</v>
       </c>
       <c r="N66">
-        <v>9.9661196357921505E-2</v>
+        <v>0.11990028072280901</v>
       </c>
       <c r="O66" t="s">
-        <v>109</v>
+        <v>2418</v>
       </c>
       <c r="P66" t="s">
-        <v>2423</v>
+        <v>2419</v>
       </c>
       <c r="Q66">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21352,19 +21375,19 @@
       </c>
       <c r="H67" s="24"/>
       <c r="L67" t="s">
-        <v>2424</v>
+        <v>2420</v>
       </c>
       <c r="M67" t="s">
-        <v>110</v>
+        <v>953</v>
       </c>
       <c r="N67">
-        <v>4.7023827138873202E-2</v>
+        <v>0.11147287996979501</v>
       </c>
       <c r="O67" t="s">
-        <v>86</v>
+        <v>464</v>
       </c>
       <c r="P67" t="s">
-        <v>2425</v>
+        <v>2421</v>
       </c>
       <c r="Q67">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21395,19 +21418,19 @@
       </c>
       <c r="H68" s="24"/>
       <c r="L68" t="s">
-        <v>2426</v>
+        <v>2422</v>
       </c>
       <c r="M68" t="s">
-        <v>2427</v>
+        <v>108</v>
       </c>
       <c r="N68">
-        <v>4.7023827138873202E-2</v>
+        <v>0.102421271752593</v>
       </c>
       <c r="O68" t="s">
-        <v>2428</v>
+        <v>109</v>
       </c>
       <c r="P68" t="s">
-        <v>2429</v>
+        <v>2423</v>
       </c>
       <c r="Q68">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21438,19 +21461,19 @@
       </c>
       <c r="H69" s="24"/>
       <c r="L69" t="s">
-        <v>2430</v>
+        <v>2424</v>
       </c>
       <c r="M69" t="s">
-        <v>2431</v>
+        <v>110</v>
       </c>
       <c r="N69">
-        <v>4.7023827138873202E-2</v>
+        <v>4.8303917799353301E-2</v>
       </c>
       <c r="O69" t="s">
-        <v>2428</v>
+        <v>86</v>
       </c>
       <c r="P69" t="s">
-        <v>2432</v>
+        <v>2425</v>
       </c>
       <c r="Q69">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21481,19 +21504,19 @@
       </c>
       <c r="H70" s="24"/>
       <c r="L70" t="s">
-        <v>2433</v>
+        <v>2426</v>
       </c>
       <c r="M70" t="s">
-        <v>111</v>
+        <v>2427</v>
       </c>
       <c r="N70">
-        <v>4.7023827138873202E-2</v>
+        <v>4.8303917799353301E-2</v>
       </c>
       <c r="O70" t="s">
-        <v>112</v>
+        <v>2428</v>
       </c>
       <c r="P70" t="s">
-        <v>2434</v>
+        <v>2429</v>
       </c>
       <c r="Q70">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21524,19 +21547,19 @@
       </c>
       <c r="H71" s="24"/>
       <c r="L71" t="s">
-        <v>2439</v>
+        <v>2430</v>
       </c>
       <c r="M71" t="s">
-        <v>2440</v>
+        <v>2431</v>
       </c>
       <c r="N71">
-        <v>4.6211448588400303E-2</v>
+        <v>4.8303917799353301E-2</v>
       </c>
       <c r="O71" t="s">
-        <v>2441</v>
+        <v>2428</v>
       </c>
       <c r="P71" t="s">
-        <v>2442</v>
+        <v>2432</v>
       </c>
       <c r="Q71">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21567,19 +21590,19 @@
       </c>
       <c r="H72" s="24"/>
       <c r="L72" t="s">
-        <v>2435</v>
+        <v>2433</v>
       </c>
       <c r="M72" t="s">
-        <v>2436</v>
+        <v>111</v>
       </c>
       <c r="N72">
-        <v>3.6075167656824697E-2</v>
+        <v>4.8303917799353301E-2</v>
       </c>
       <c r="O72" t="s">
-        <v>2437</v>
+        <v>112</v>
       </c>
       <c r="P72" t="s">
-        <v>2438</v>
+        <v>2434</v>
       </c>
       <c r="Q72">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21610,23 +21633,23 @@
       </c>
       <c r="H73" s="24"/>
       <c r="L73" t="s">
-        <v>1995</v>
+        <v>2439</v>
       </c>
       <c r="M73" t="s">
-        <v>869</v>
+        <v>2440</v>
       </c>
       <c r="N73" s="1">
-        <v>0</v>
+        <v>4.6793501262688303E-2</v>
       </c>
       <c r="O73" t="s">
-        <v>870</v>
+        <v>2441</v>
       </c>
       <c r="P73" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="Q73">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:17">
@@ -21653,19 +21676,19 @@
       </c>
       <c r="H74" s="24"/>
       <c r="L74" t="s">
-        <v>2444</v>
+        <v>2435</v>
       </c>
       <c r="M74" t="s">
-        <v>1067</v>
+        <v>2436</v>
       </c>
       <c r="N74" s="1">
-        <v>0</v>
+        <v>3.7057212037354903E-2</v>
       </c>
       <c r="O74" t="s">
-        <v>2445</v>
+        <v>2437</v>
       </c>
       <c r="P74" t="s">
-        <v>2446</v>
+        <v>2438</v>
       </c>
       <c r="Q74">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21696,23 +21719,23 @@
       </c>
       <c r="H75" s="24"/>
       <c r="L75" t="s">
-        <v>2010</v>
+        <v>1995</v>
       </c>
       <c r="M75" t="s">
-        <v>26</v>
+        <v>869</v>
       </c>
       <c r="N75" s="1">
         <v>0</v>
       </c>
       <c r="O75" t="s">
-        <v>2009</v>
+        <v>870</v>
       </c>
       <c r="P75" t="s">
-        <v>2415</v>
+        <v>2443</v>
       </c>
       <c r="Q75">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:17">
@@ -21739,23 +21762,23 @@
       </c>
       <c r="H76" s="24"/>
       <c r="L76" t="s">
-        <v>1759</v>
+        <v>2444</v>
       </c>
       <c r="M76" t="s">
-        <v>118</v>
+        <v>1067</v>
       </c>
       <c r="N76" s="1">
         <v>0</v>
       </c>
       <c r="O76" t="s">
-        <v>1756</v>
+        <v>2445</v>
       </c>
       <c r="P76" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="Q76">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:17">
@@ -21782,23 +21805,23 @@
       </c>
       <c r="H77" s="24"/>
       <c r="L77" t="s">
-        <v>2448</v>
+        <v>2010</v>
       </c>
       <c r="M77" t="s">
-        <v>2436</v>
+        <v>26</v>
       </c>
       <c r="N77" s="1">
         <v>0</v>
       </c>
       <c r="O77" t="s">
-        <v>2437</v>
+        <v>2009</v>
       </c>
       <c r="P77" t="s">
-        <v>2449</v>
+        <v>2415</v>
       </c>
       <c r="Q77">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:17">
@@ -21825,23 +21848,23 @@
       </c>
       <c r="H78" s="24"/>
       <c r="L78" t="s">
-        <v>2450</v>
+        <v>1759</v>
       </c>
       <c r="M78" t="s">
-        <v>2451</v>
+        <v>118</v>
       </c>
       <c r="N78" s="1">
         <v>0</v>
       </c>
       <c r="O78" t="s">
-        <v>2437</v>
+        <v>1756</v>
       </c>
       <c r="P78" t="s">
-        <v>2452</v>
+        <v>2447</v>
       </c>
       <c r="Q78">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:17">
@@ -21868,23 +21891,23 @@
       </c>
       <c r="H79" s="24"/>
       <c r="L79" t="s">
-        <v>2033</v>
+        <v>2448</v>
       </c>
       <c r="M79" t="s">
-        <v>1050</v>
+        <v>2436</v>
       </c>
       <c r="N79" s="1">
         <v>0</v>
       </c>
       <c r="O79" t="s">
-        <v>482</v>
+        <v>2437</v>
       </c>
       <c r="P79" t="s">
-        <v>2453</v>
+        <v>2449</v>
       </c>
       <c r="Q79">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -21911,19 +21934,19 @@
       </c>
       <c r="H80" s="24"/>
       <c r="L80" t="s">
-        <v>2454</v>
+        <v>2450</v>
       </c>
       <c r="M80" t="s">
-        <v>106</v>
+        <v>2451</v>
       </c>
       <c r="N80" s="1">
         <v>0</v>
       </c>
       <c r="O80" t="s">
-        <v>107</v>
+        <v>2437</v>
       </c>
       <c r="P80" t="s">
-        <v>2455</v>
+        <v>2452</v>
       </c>
       <c r="Q80">
         <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
@@ -21953,7 +21976,25 @@
         <v>8.6257E-2</v>
       </c>
       <c r="H81" s="24"/>
-      <c r="N81" s="1"/>
+      <c r="L81" t="s">
+        <v>2033</v>
+      </c>
+      <c r="M81" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N81" s="1">
+        <v>0</v>
+      </c>
+      <c r="O81" t="s">
+        <v>482</v>
+      </c>
+      <c r="P81" t="s">
+        <v>2453</v>
+      </c>
+      <c r="Q81" s="33">
+        <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="82" spans="1:22">
       <c r="A82" s="24" t="s">
@@ -21978,7 +22019,25 @@
         <v>8.6257E-2</v>
       </c>
       <c r="H82" s="24"/>
-      <c r="N82" s="1"/>
+      <c r="L82" t="s">
+        <v>2454</v>
+      </c>
+      <c r="M82" t="s">
+        <v>106</v>
+      </c>
+      <c r="N82" s="1">
+        <v>0</v>
+      </c>
+      <c r="O82" t="s">
+        <v>107</v>
+      </c>
+      <c r="P82" t="s">
+        <v>2455</v>
+      </c>
+      <c r="Q82" s="33">
+        <f>COUNTIF(Tabela4[geneID],Tabela5[[#This Row],[grRules]])</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="83" spans="1:22">
       <c r="A83" s="24" t="s">
@@ -30363,7 +30422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA629B35-2757-48F7-9C36-0B4946EA8231}">
   <dimension ref="A1:E361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -36295,7 +36354,7 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>